<commit_message>
Added possible analysis topics
</commit_message>
<xml_diff>
--- a/Survey Spreadsheets/Factors of Academic Success Survey (1.01).xlsx
+++ b/Survey Spreadsheets/Factors of Academic Success Survey (1.01).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis\Documents\Factors of Academic Success\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis\Documents\Git\Factors of Academic Success\Survey Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0B8317-753C-41CB-BB05-3FA0D5B7D4DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98ADF88-364B-45C4-87CB-058A8BE38B5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -802,21 +802,6 @@
     <t>UP_FROM_BED</t>
   </si>
   <si>
-    <t>F_OPENESS</t>
-  </si>
-  <si>
-    <t>F_CONSCIENTIOUSNESS</t>
-  </si>
-  <si>
-    <t>F_EXTRAVERSION</t>
-  </si>
-  <si>
-    <t>F_AGREEABLENESS</t>
-  </si>
-  <si>
-    <t>F_NEUROTICISM</t>
-  </si>
-  <si>
     <t>MYERS_BRIGGS</t>
   </si>
   <si>
@@ -851,6 +836,21 @@
   </si>
   <si>
     <t>SHOW_UP_EARLY</t>
+  </si>
+  <si>
+    <t>OPENESS</t>
+  </si>
+  <si>
+    <t>CONSCIENTIOUSNESS</t>
+  </si>
+  <si>
+    <t>EXTRAVERSION</t>
+  </si>
+  <si>
+    <t>AGREEABLENESS</t>
+  </si>
+  <si>
+    <t>NEUROTICISM</t>
   </si>
 </sst>
 </file>
@@ -1119,9 +1119,9 @@
   </sheetPr>
   <dimension ref="A1:AO28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP8" sqref="AP8"/>
+      <selection pane="bottomLeft" activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1131,10 +1131,10 @@
   <sheetData>
     <row r="1" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>239</v>
@@ -1185,7 +1185,7 @@
         <v>254</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>255</v>
@@ -1203,46 +1203,46 @@
         <v>259</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>

</xml_diff>

<commit_message>
Converted ACT to SAT
</commit_message>
<xml_diff>
--- a/Survey Spreadsheets/Factors of Academic Success Survey (1.01).xlsx
+++ b/Survey Spreadsheets/Factors of Academic Success Survey (1.01).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis\Documents\Git\Factors of Academic Success\Survey Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98ADF88-364B-45C4-87CB-058A8BE38B5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C502A4A-9572-4329-BC0A-04E4FC98F2F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -838,9 +838,6 @@
     <t>SHOW_UP_EARLY</t>
   </si>
   <si>
-    <t>OPENESS</t>
-  </si>
-  <si>
     <t>CONSCIENTIOUSNESS</t>
   </si>
   <si>
@@ -851,6 +848,9 @@
   </si>
   <si>
     <t>NEUROTICISM</t>
+  </si>
+  <si>
+    <t>OPENNESS</t>
   </si>
 </sst>
 </file>
@@ -1119,9 +1119,9 @@
   </sheetPr>
   <dimension ref="A1:AO28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC3" sqref="AC3"/>
+      <selection pane="bottomLeft" activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1203,19 +1203,19 @@
         <v>259</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>260</v>

</xml_diff>